<commit_message>
added missing experiment source ID
</commit_message>
<xml_diff>
--- a/EGA_metadata_forms.xlsx
+++ b/EGA_metadata_forms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7020" tabRatio="776" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7020" tabRatio="776" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="356">
   <si>
     <t>alias</t>
   </si>
@@ -1179,12 +1179,31 @@
   <si>
     <t>date when file was generated</t>
   </si>
+  <si>
+    <t>GENOMIC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It is possible to add any custom attributes using colon-separated tag, value pairs using the format </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>attributes:tag:value</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1264,6 +1283,14 @@
     <font>
       <b/>
       <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2017,8 +2044,8 @@
       <c r="B10"/>
     </row>
     <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>79</v>
+      <c r="A11" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="B11"/>
     </row>
@@ -2234,9 +2261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2572,19 +2597,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'EGA controlled vocabulary'!$A$177:$A$178</xm:f>
+            <xm:f>'EGA controlled vocabulary'!$A$178:$A$179</xm:f>
           </x14:formula1>
           <xm:sqref>B20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'EGA controlled vocabulary'!$A$179:$A$181</xm:f>
+            <xm:f>'EGA controlled vocabulary'!$A$180:$A$182</xm:f>
           </x14:formula1>
           <xm:sqref>B29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'EGA controlled vocabulary'!$A$182:$A$186</xm:f>
+            <xm:f>'EGA controlled vocabulary'!$A$183:$A$187</xm:f>
           </x14:formula1>
           <xm:sqref>B30</xm:sqref>
         </x14:dataValidation>
@@ -2794,7 +2819,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'EGA controlled vocabulary'!$A$175:$A$176</xm:f>
+            <xm:f>'EGA controlled vocabulary'!$A$176:$A$177</xm:f>
           </x14:formula1>
           <xm:sqref>B11</xm:sqref>
         </x14:dataValidation>
@@ -3173,19 +3198,19 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'EGA controlled vocabulary'!$A$70:$A$77</xm:f>
+            <xm:f>'EGA controlled vocabulary'!$A$70:$A$78</xm:f>
           </x14:formula1>
           <xm:sqref>B33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'EGA controlled vocabulary'!$A$78:$A$113</xm:f>
+            <xm:f>'EGA controlled vocabulary'!$A$79:$A$114</xm:f>
           </x14:formula1>
           <xm:sqref>B34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'EGA controlled vocabulary'!$A$114:$A$174</xm:f>
+            <xm:f>'EGA controlled vocabulary'!$A$115:$A$175</xm:f>
           </x14:formula1>
           <xm:sqref>B30</xm:sqref>
         </x14:dataValidation>
@@ -3328,9 +3353,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B186"/>
+  <dimension ref="A1:B187"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3889,7 +3916,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>354</v>
       </c>
       <c r="B70" t="s">
         <v>170</v>
@@ -3897,7 +3924,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B71" t="s">
         <v>170</v>
@@ -3905,7 +3932,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B72" t="s">
         <v>170</v>
@@ -3913,7 +3940,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B73" t="s">
         <v>170</v>
@@ -3921,7 +3948,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B74" t="s">
         <v>170</v>
@@ -3929,7 +3956,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B75" t="s">
         <v>170</v>
@@ -3937,7 +3964,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B76" t="s">
         <v>170</v>
@@ -3945,7 +3972,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B77" t="s">
         <v>170</v>
@@ -3953,15 +3980,15 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B78" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B79" t="s">
         <v>214</v>
@@ -3969,7 +3996,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B80" t="s">
         <v>214</v>
@@ -3977,7 +4004,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B81" t="s">
         <v>214</v>
@@ -3985,7 +4012,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B82" t="s">
         <v>214</v>
@@ -3993,7 +4020,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B83" t="s">
         <v>214</v>
@@ -4001,7 +4028,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B84" t="s">
         <v>214</v>
@@ -4009,7 +4036,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="B85" t="s">
         <v>214</v>
@@ -4017,7 +4044,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>187</v>
+        <v>142</v>
       </c>
       <c r="B86" t="s">
         <v>214</v>
@@ -4025,7 +4052,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B87" t="s">
         <v>214</v>
@@ -4033,7 +4060,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B88" t="s">
         <v>214</v>
@@ -4041,7 +4068,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B89" t="s">
         <v>214</v>
@@ -4049,7 +4076,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B90" t="s">
         <v>214</v>
@@ -4057,7 +4084,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B91" t="s">
         <v>214</v>
@@ -4065,7 +4092,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B92" t="s">
         <v>214</v>
@@ -4073,7 +4100,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B93" t="s">
         <v>214</v>
@@ -4081,7 +4108,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B94" t="s">
         <v>214</v>
@@ -4089,7 +4116,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B95" t="s">
         <v>214</v>
@@ -4097,7 +4124,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="B96" t="s">
         <v>214</v>
@@ -4105,7 +4132,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
         <v>214</v>
@@ -4113,7 +4140,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B98" t="s">
         <v>214</v>
@@ -4121,7 +4148,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B99" t="s">
         <v>214</v>
@@ -4129,7 +4156,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B100" t="s">
         <v>214</v>
@@ -4137,7 +4164,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B101" t="s">
         <v>214</v>
@@ -4145,7 +4172,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B102" t="s">
         <v>214</v>
@@ -4153,7 +4180,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B103" t="s">
         <v>214</v>
@@ -4161,7 +4188,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B104" t="s">
         <v>214</v>
@@ -4169,7 +4196,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B105" t="s">
         <v>214</v>
@@ -4177,7 +4204,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B106" t="s">
         <v>214</v>
@@ -4185,7 +4212,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B107" t="s">
         <v>214</v>
@@ -4193,7 +4220,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B108" t="s">
         <v>214</v>
@@ -4201,7 +4228,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B109" t="s">
         <v>214</v>
@@ -4209,7 +4236,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B110" t="s">
         <v>214</v>
@@ -4217,7 +4244,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B111" t="s">
         <v>214</v>
@@ -4225,7 +4252,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B112" t="s">
         <v>214</v>
@@ -4233,7 +4260,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B113" t="s">
         <v>214</v>
@@ -4241,15 +4268,15 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B114" t="s">
-        <v>276</v>
+        <v>214</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B115" t="s">
         <v>276</v>
@@ -4257,7 +4284,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B116" t="s">
         <v>276</v>
@@ -4265,7 +4292,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B117" t="s">
         <v>276</v>
@@ -4273,7 +4300,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B118" t="s">
         <v>276</v>
@@ -4281,7 +4308,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B119" t="s">
         <v>276</v>
@@ -4289,7 +4316,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B120" t="s">
         <v>276</v>
@@ -4297,7 +4324,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B121" t="s">
         <v>276</v>
@@ -4305,7 +4332,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B122" t="s">
         <v>276</v>
@@ -4313,7 +4340,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B123" t="s">
         <v>276</v>
@@ -4321,7 +4348,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B124" t="s">
         <v>276</v>
@@ -4329,7 +4356,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B125" t="s">
         <v>276</v>
@@ -4337,7 +4364,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B126" t="s">
         <v>276</v>
@@ -4345,7 +4372,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B127" t="s">
         <v>276</v>
@@ -4353,7 +4380,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B128" t="s">
         <v>276</v>
@@ -4361,7 +4388,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B129" t="s">
         <v>276</v>
@@ -4369,7 +4396,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B130" t="s">
         <v>276</v>
@@ -4377,7 +4404,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B131" t="s">
         <v>276</v>
@@ -4385,7 +4412,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B132" t="s">
         <v>276</v>
@@ -4393,7 +4420,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B133" t="s">
         <v>276</v>
@@ -4401,7 +4428,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B134" t="s">
         <v>276</v>
@@ -4409,7 +4436,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B135" t="s">
         <v>276</v>
@@ -4417,7 +4444,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B136" t="s">
         <v>276</v>
@@ -4425,7 +4452,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B137" t="s">
         <v>276</v>
@@ -4433,7 +4460,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B138" t="s">
         <v>276</v>
@@ -4441,7 +4468,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B139" t="s">
         <v>276</v>
@@ -4449,7 +4476,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B140" t="s">
         <v>276</v>
@@ -4457,7 +4484,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B141" t="s">
         <v>276</v>
@@ -4465,7 +4492,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B142" t="s">
         <v>276</v>
@@ -4473,7 +4500,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B143" t="s">
         <v>276</v>
@@ -4481,7 +4508,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B144" t="s">
         <v>276</v>
@@ -4489,7 +4516,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B145" t="s">
         <v>276</v>
@@ -4497,7 +4524,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B146" t="s">
         <v>276</v>
@@ -4505,7 +4532,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B147" t="s">
         <v>276</v>
@@ -4513,7 +4540,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B148" t="s">
         <v>276</v>
@@ -4521,7 +4548,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B149" t="s">
         <v>276</v>
@@ -4529,7 +4556,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B150" t="s">
         <v>276</v>
@@ -4537,7 +4564,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B151" t="s">
         <v>276</v>
@@ -4545,7 +4572,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B152" t="s">
         <v>276</v>
@@ -4553,7 +4580,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B153" t="s">
         <v>276</v>
@@ -4561,7 +4588,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B154" t="s">
         <v>276</v>
@@ -4569,7 +4596,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B155" t="s">
         <v>276</v>
@@ -4577,7 +4604,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B156" t="s">
         <v>276</v>
@@ -4585,7 +4612,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B157" t="s">
         <v>276</v>
@@ -4593,7 +4620,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B158" t="s">
         <v>276</v>
@@ -4601,7 +4628,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B159" t="s">
         <v>276</v>
@@ -4609,7 +4636,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B160" t="s">
         <v>276</v>
@@ -4617,7 +4644,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B161" t="s">
         <v>276</v>
@@ -4625,7 +4652,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B162" t="s">
         <v>276</v>
@@ -4633,7 +4660,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B163" t="s">
         <v>276</v>
@@ -4641,7 +4668,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B164" t="s">
         <v>276</v>
@@ -4649,7 +4676,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B165" t="s">
         <v>276</v>
@@ -4657,7 +4684,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B166" t="s">
         <v>276</v>
@@ -4665,7 +4692,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B167" t="s">
         <v>276</v>
@@ -4673,7 +4700,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B168" t="s">
         <v>276</v>
@@ -4681,7 +4708,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B169" t="s">
         <v>276</v>
@@ -4689,7 +4716,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B170" t="s">
         <v>276</v>
@@ -4697,7 +4724,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B171" t="s">
         <v>276</v>
@@ -4705,7 +4732,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B172" t="s">
         <v>276</v>
@@ -4713,7 +4740,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B173" t="s">
         <v>276</v>
@@ -4721,7 +4748,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B174" t="s">
         <v>276</v>
@@ -4729,15 +4756,15 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="B175" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B176" t="s">
         <v>298</v>
@@ -4745,15 +4772,15 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>324</v>
+        <v>297</v>
       </c>
       <c r="B177" t="s">
-        <v>326</v>
+        <v>298</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B178" t="s">
         <v>326</v>
@@ -4761,15 +4788,15 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B179" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B180" t="s">
         <v>338</v>
@@ -4777,7 +4804,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B181" t="s">
         <v>338</v>
@@ -4785,15 +4812,15 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B182" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>103</v>
+        <v>340</v>
       </c>
       <c r="B183" t="s">
         <v>342</v>
@@ -4801,7 +4828,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B184" t="s">
         <v>342</v>
@@ -4809,7 +4836,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>331</v>
+        <v>105</v>
       </c>
       <c r="B185" t="s">
         <v>342</v>
@@ -4817,9 +4844,17 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
+        <v>331</v>
+      </c>
+      <c r="B186" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
         <v>341</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B187" t="s">
         <v>342</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed custom sample fields
</commit_message>
<xml_diff>
--- a/EGA_metadata_forms.xlsx
+++ b/EGA_metadata_forms.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjovelin\Desktop\Gaea\Gaea\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjovelin\Desktop\Gaea\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AB7DE9-ADA5-4F43-9CEB-70288203EE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7020" tabRatio="776" activeTab="8"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="346">
   <si>
     <t>alias</t>
   </si>
@@ -280,22 +281,7 @@
     <t>sample phenotype</t>
   </si>
   <si>
-    <t>Please complete the following sample attributes</t>
-  </si>
-  <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>Sample attributes are assigned to all samples.</t>
-  </si>
-  <si>
-    <t>It is required to split samples into subsets if different attributes must be associated to groups of samples.</t>
-  </si>
-  <si>
-    <t>1) Create new sample tabs for each group of samples</t>
-  </si>
-  <si>
-    <t>2) Provide sample attribute information for each group of samples</t>
   </si>
   <si>
     <r>
@@ -320,38 +306,6 @@
     <t>Please complete the following sample information</t>
   </si>
   <si>
-    <t>attributes:origin:Canada</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For instance, add the following lines below </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>description</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to specify the subjects origin and age:</t>
-    </r>
-  </si>
-  <si>
-    <t>attributes:age:70</t>
-  </si>
-  <si>
     <t>To add more samples to the table below:</t>
   </si>
   <si>
@@ -461,9 +415,6 @@
   </si>
   <si>
     <t>3) Fill in the experiment table for each group of experiments</t>
-  </si>
-  <si>
-    <t>3) Fill in the sample table for each group of samples</t>
   </si>
   <si>
     <t>study accession</t>
@@ -1182,28 +1133,12 @@
   <si>
     <t>GENOMIC</t>
   </si>
-  <si>
-    <r>
-      <t xml:space="preserve">It is possible to add any custom attributes using colon-separated tag, value pairs using the format </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attributes:tag:value</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1287,14 +1222,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1316,18 +1243,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1610,8 +1533,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -1623,7 +1546,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1677,53 +1600,44 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B19" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1731,7 +1645,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$2:$A$17</xm:f>
           </x14:formula1>
@@ -1744,7 +1658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1759,7 +1673,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1813,46 +1727,46 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1863,7 +1777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1875,12 +1789,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1927,37 +1841,37 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -1980,10 +1894,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1993,245 +1909,159 @@
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:4" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B3"/>
-    </row>
-    <row r="4" spans="1:4" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A4" s="5"/>
-      <c r="B4"/>
-    </row>
-    <row r="5" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>77</v>
       </c>
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>78</v>
       </c>
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10"/>
-      <c r="B10"/>
-    </row>
-    <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="B11"/>
-    </row>
-    <row r="12" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13"/>
-    </row>
-    <row r="14" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>80</v>
       </c>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.4">
+      <c r="A26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A18" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="B27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A21" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A22" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="10"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A39" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2239,17 +2069,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$18:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>C40</xm:sqref>
+          <xm:sqref>C27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$21:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>B40</xm:sqref>
+          <xm:sqref>B27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2258,7 +2088,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2272,188 +2102,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:1" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A20" s="9" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-    </row>
-    <row r="5" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A23" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A26" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A27" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A28" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B28" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A29" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B29" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A30" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B30" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A18" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A19" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A20" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
-    </row>
-    <row r="22" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="23" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A23" s="5" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24"/>
-    </row>
-    <row r="25" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25"/>
-    </row>
-    <row r="26" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A26" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A27" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A28" s="9" t="s">
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.4">
+      <c r="A33" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A29" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A30" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31"/>
-    </row>
-    <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32"/>
-    </row>
-    <row r="33" spans="1:5" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A33" s="5" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A34" s="5" t="s">
+    </row>
+    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.4">
+      <c r="A34" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
@@ -2471,123 +2285,123 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C37" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B38" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C38" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B39" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="C39" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B40" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C40" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B41" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C41" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A43" s="5" t="s">
-        <v>312</v>
+      <c r="A43" s="4" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>347</v>
+      <c r="B45" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>348</v>
+      <c r="D46" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>348</v>
+      <c r="D47" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2595,19 +2409,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$178:$A$179</xm:f>
           </x14:formula1>
           <xm:sqref>B20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$180:$A$182</xm:f>
           </x14:formula1>
           <xm:sqref>B29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000002000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$183:$A$187</xm:f>
           </x14:formula1>
@@ -2620,10 +2434,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2634,46 +2450,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
-        <v>289</v>
+      <c r="A1" s="2" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
-        <v>290</v>
+      <c r="A3" s="4" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A4" s="5"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A11" s="9" t="s">
-        <v>295</v>
+      <c r="A11" s="5" t="s">
+        <v>286</v>
       </c>
       <c r="B11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C11" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2693,123 +2509,106 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="C15" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B16" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C16" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B17" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C17" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B18" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C18" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>307</v>
-      </c>
-      <c r="B19" t="s">
-        <v>309</v>
-      </c>
-      <c r="C19" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A21" s="5" t="s">
-        <v>312</v>
+      <c r="A21" s="4" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A24" s="5" t="s">
-        <v>290</v>
+      <c r="A24" s="4" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.4">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>307</v>
-      </c>
+      <c r="B28" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2817,7 +2616,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$176:$A$177</xm:f>
           </x14:formula1>
@@ -2830,7 +2629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2843,41 +2642,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
-        <v>115</v>
+      <c r="A1" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
-        <v>116</v>
+      <c r="A3" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A4" s="5"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -2896,60 +2695,60 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" t="s">
         <v>123</v>
       </c>
-      <c r="B14" t="s">
-        <v>132</v>
-      </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
         <v>65</v>
@@ -2957,21 +2756,21 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
         <v>65</v>
@@ -2979,10 +2778,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
         <v>65</v>
@@ -2990,225 +2789,225 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A28" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A29" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="A29" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A30" s="9" t="s">
-        <v>125</v>
+      <c r="A30" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>238</v>
-      </c>
-      <c r="C30" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A31" s="9" t="s">
-        <v>126</v>
+      <c r="A31" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C31" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A32" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A33" s="9" t="s">
-        <v>130</v>
+      <c r="A33" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>177</v>
-      </c>
-      <c r="C33" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A34" s="9" t="s">
-        <v>131</v>
+      <c r="A34" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>209</v>
-      </c>
-      <c r="C34" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A35" s="9" t="s">
-        <v>137</v>
+      <c r="A35" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A36" s="9"/>
-      <c r="C36" s="8"/>
+      <c r="A36" s="5"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A37" s="9"/>
-      <c r="C37" s="8"/>
+      <c r="A37" s="5"/>
+      <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A38" s="5" t="s">
-        <v>284</v>
+      <c r="A38" s="4" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A40" s="5"/>
+      <c r="A40" s="4"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="C41" s="12" t="s">
+      <c r="B41" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="11" t="s">
-        <v>281</v>
+      <c r="A42" s="7" t="s">
+        <v>272</v>
       </c>
       <c r="B42" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C42" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:3" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.4">
-      <c r="A47" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="B47" s="13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:3" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.4">
+      <c r="A47" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
+      <c r="C47" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$37:$A$38</xm:f>
           </x14:formula1>
           <xm:sqref>B35:B37</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$39:$A$69</xm:f>
           </x14:formula1>
           <xm:sqref>B31</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000002000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$70:$A$78</xm:f>
           </x14:formula1>
           <xm:sqref>B33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000003000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$79:$A$114</xm:f>
           </x14:formula1>
           <xm:sqref>B34</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000004000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$115:$A$175</xm:f>
           </x14:formula1>
@@ -3221,7 +3020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -3234,8 +3033,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
-        <v>92</v>
+      <c r="A1" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -3250,86 +3049,86 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" t="s">
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>74</v>
+      <c r="A6" t="s">
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>93</v>
+      <c r="A7" t="s">
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A13" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.5">
-      <c r="A14" s="9" t="s">
-        <v>93</v>
+      <c r="A14" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3339,7 +3138,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
           <x14:formula1>
             <xm:f>'EGA controlled vocabulary'!$A$23:$A$36</xm:f>
           </x14:formula1>
@@ -3352,10 +3151,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+    <sheetView topLeftCell="A99" workbookViewId="0">
       <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
@@ -3540,114 +3339,114 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" t="s">
         <v>106</v>
-      </c>
-      <c r="B29" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -3655,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -3663,1199 +3462,1199 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B49" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B53" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B55" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B60" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B61" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" t="s">
         <v>162</v>
-      </c>
-      <c r="B62" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B64" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B65" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B66" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B67" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B68" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B69" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B70" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B71" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B72" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B73" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B74" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B75" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B76" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B77" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B78" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B80" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B81" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B82" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B83" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B84" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B85" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B86" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B87" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B88" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B89" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B90" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B91" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B92" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B93" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B94" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B95" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B96" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B97" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B98" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B99" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B101" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B102" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B104" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B105" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>196</v>
+      </c>
+      <c r="B106" t="s">
         <v>205</v>
-      </c>
-      <c r="B106" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B107" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B109" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B110" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B111" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B112" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B113" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B114" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B115" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B116" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B117" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B118" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B119" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B120" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B121" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B122" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B123" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B124" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B125" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B126" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B127" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B128" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B129" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B130" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B131" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B132" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B133" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B134" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B135" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B136" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B137" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B138" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B139" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B140" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B141" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B142" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B143" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B144" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B145" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B146" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B147" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B148" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B149" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B150" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B151" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B152" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B153" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B154" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B155" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B156" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B157" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B158" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B159" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B160" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B161" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B162" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B163" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B164" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B165" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B166" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B167" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B168" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B169" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B170" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B171" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B172" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B173" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B174" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B175" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B176" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B177" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B178" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B179" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B180" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B181" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B182" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B183" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B184" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B185" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B186" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B187" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>